<commit_message>
Dobbelsteen toegevoegd en werkend
</commit_message>
<xml_diff>
--- a/Documenten/final Sprint 2 backlog & product backlog overview.xlsx
+++ b/Documenten/final Sprint 2 backlog & product backlog overview.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Desktop\Project-2-Game-Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Desktop\Project-2-Game-Development\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -408,13 +408,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
@@ -715,10 +715,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="9"/>
@@ -1032,7 +1032,7 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="26" t="s">
         <v>55</v>
       </c>
       <c r="E14" s="9"/>
@@ -1056,7 +1056,7 @@
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="9"/>
@@ -1093,7 +1093,7 @@
       <c r="C17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="9"/>
@@ -1117,7 +1117,7 @@
       <c r="C18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="9"/>
@@ -1141,7 +1141,7 @@
       <c r="C19" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="9"/>
@@ -1165,7 +1165,7 @@
       <c r="C20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E20" s="9"/>
@@ -1189,7 +1189,7 @@
       <c r="C21" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="9"/>
@@ -1213,7 +1213,7 @@
       <c r="C22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="9"/>
@@ -1237,7 +1237,7 @@
       <c r="C23" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="9"/>
@@ -1261,7 +1261,7 @@
       <c r="C24" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="9"/>
@@ -1285,7 +1285,7 @@
       <c r="C25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="9"/>
@@ -16913,8 +16913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16928,10 +16928,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -17048,7 +17048,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="12">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>17</v>

</xml_diff>